<commit_message>
HW-118 Charger Interface Rev 3 - Added teardrops to PCB - Generated output files
</commit_message>
<xml_diff>
--- a/MSXII_ChargerInterface/Project Outputs for MSXII_ChargerInterface/MSXII_ChargerInterface_3.0.xlsx
+++ b/MSXII_ChargerInterface/Project Outputs for MSXII_ChargerInterface/MSXII_ChargerInterface_3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiping\Documents\Midnight Sun\hardware\MSXII_ChargerInterface\Project Outputs for MSXII_ChargerInterface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A5B19C5-D14B-4756-B9D2-51B33B8240D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A7A8EB-3E1E-45C9-9AC2-CA8A17CF4114}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="4215" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -1244,7 +1244,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="31">
-        <v>43541.731944444444</v>
+        <v>43542.470138888886</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -2390,7 +2390,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="32">
-        <v>0.7319444444444444</v>
+        <v>0.47013888888888888</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2398,7 +2398,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="33">
-        <v>43541</v>
+        <v>43542</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2406,7 +2406,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="34">
-        <v>43541.731944444444</v>
+        <v>43542.470138888886</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>